<commit_message>
Mejora visual del proyecto y ajustes en lógica de ventas
</commit_message>
<xml_diff>
--- a/data/inventario.xlsx
+++ b/data/inventario.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,10 +416,10 @@
         <v>precio</v>
       </c>
       <c r="E1" t="str">
+        <v>costo</v>
+      </c>
+      <c r="F1" t="str">
         <v>fecha_registro</v>
-      </c>
-      <c r="F1" t="str">
-        <v>costo</v>
       </c>
     </row>
     <row r="2">
@@ -430,61 +430,21 @@
         <v>Aguardientes</v>
       </c>
       <c r="C2">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D2">
         <v>108000</v>
       </c>
-      <c r="E2" t="str">
-        <v>24/1/2026</v>
-      </c>
-      <c r="F2">
-        <v>58000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Aguardiente Amarillo Media</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Aguardientes</v>
-      </c>
-      <c r="C3">
-        <v>1000</v>
-      </c>
-      <c r="D3">
+      <c r="E2">
         <v>78000</v>
       </c>
-      <c r="E3" t="str">
-        <v>24/1/2026</v>
-      </c>
-      <c r="F3">
-        <v>38000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Cerveza Corona</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Cervezas</v>
-      </c>
-      <c r="C4">
-        <v>1000</v>
-      </c>
-      <c r="D4">
-        <v>10000</v>
-      </c>
-      <c r="E4" t="str">
-        <v>26/1/2026</v>
-      </c>
-      <c r="F4">
-        <v>5000</v>
+      <c r="F2" t="str">
+        <v>31/1/2026</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mejora visual de inconos y resolucion de problemas para las accesiones de agregar, modificar y eliminar usuarios
</commit_message>
<xml_diff>
--- a/data/inventario.xlsx
+++ b/data/inventario.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,10 +416,10 @@
         <v>precio</v>
       </c>
       <c r="E1" t="str">
+        <v>fecha_registro</v>
+      </c>
+      <c r="F1" t="str">
         <v>costo</v>
-      </c>
-      <c r="F1" t="str">
-        <v>fecha_registro</v>
       </c>
     </row>
     <row r="2">
@@ -430,21 +430,41 @@
         <v>Aguardientes</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="D2">
         <v>108000</v>
       </c>
-      <c r="E2">
-        <v>78000</v>
-      </c>
-      <c r="F2" t="str">
+      <c r="E2" t="str">
         <v>31/1/2026</v>
+      </c>
+      <c r="F2">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Cerveza Corona</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Cervezas</v>
+      </c>
+      <c r="C3">
+        <v>996</v>
+      </c>
+      <c r="D3">
+        <v>10000</v>
+      </c>
+      <c r="E3" t="str">
+        <v>31/1/2026</v>
+      </c>
+      <c r="F3">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se repara fallo en el Js de ventas, no se veian imagenes con caracteres especiales
</commit_message>
<xml_diff>
--- a/data/inventario.xlsx
+++ b/data/inventario.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,7 +430,7 @@
         <v>Aguardientes</v>
       </c>
       <c r="C2">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="D2">
         <v>108000</v>
@@ -450,7 +450,7 @@
         <v>Cervezas</v>
       </c>
       <c r="C3">
-        <v>996</v>
+        <v>988</v>
       </c>
       <c r="D3">
         <v>10000</v>
@@ -460,11 +460,31 @@
       </c>
       <c r="F3">
         <v>5000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Ron viejo de caldas (5años) botella</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Rones</v>
+      </c>
+      <c r="C4">
+        <v>999</v>
+      </c>
+      <c r="D4">
+        <v>132000</v>
+      </c>
+      <c r="E4" t="str">
+        <v>3/2/2026</v>
+      </c>
+      <c r="F4">
+        <v>78000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificacion de boton de ventas, colores y fondo
</commit_message>
<xml_diff>
--- a/data/inventario.xlsx
+++ b/data/inventario.xlsx
@@ -430,7 +430,7 @@
         <v>Aguardientes</v>
       </c>
       <c r="C2">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="D2">
         <v>108000</v>
@@ -450,7 +450,7 @@
         <v>Cervezas</v>
       </c>
       <c r="C3">
-        <v>988</v>
+        <v>981</v>
       </c>
       <c r="D3">
         <v>10000</v>
@@ -470,7 +470,7 @@
         <v>Rones</v>
       </c>
       <c r="C4">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="D4">
         <v>132000</v>

</xml_diff>

<commit_message>
En inventario se cre una pestaña con aviso y modal para ventas nuevas, adicional se modifica el login
</commit_message>
<xml_diff>
--- a/data/inventario.xlsx
+++ b/data/inventario.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,67 +424,87 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Aguardiente Amarillo Botella</v>
+        <v>Cerveza Corona</v>
       </c>
       <c r="B2" t="str">
-        <v>Aguardientes</v>
+        <v>Cervezas</v>
       </c>
       <c r="C2">
-        <v>991</v>
+        <v>982</v>
       </c>
       <c r="D2">
-        <v>108000</v>
+        <v>10000</v>
       </c>
       <c r="E2" t="str">
         <v>31/1/2026</v>
       </c>
       <c r="F2">
-        <v>45000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Cerveza Corona</v>
+        <v>Ron viejo de caldas (5años) botella</v>
       </c>
       <c r="B3" t="str">
-        <v>Cervezas</v>
+        <v>Rones</v>
       </c>
       <c r="C3">
-        <v>981</v>
+        <v>999</v>
       </c>
       <c r="D3">
-        <v>10000</v>
+        <v>132000</v>
       </c>
       <c r="E3" t="str">
-        <v>31/1/2026</v>
+        <v>3/2/2026</v>
       </c>
       <c r="F3">
-        <v>5000</v>
+        <v>78000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Ron viejo de caldas (5años) botella</v>
+        <v>Aguardiente Amarillo Media</v>
       </c>
       <c r="B4" t="str">
-        <v>Rones</v>
+        <v>Aguardientes</v>
       </c>
       <c r="C4">
-        <v>996</v>
+        <v>119</v>
       </c>
       <c r="D4">
-        <v>132000</v>
+        <v>70000</v>
       </c>
       <c r="E4" t="str">
-        <v>3/2/2026</v>
+        <v>6/2/2026</v>
       </c>
       <c r="F4">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Aguardiente Amarillo Botella</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Aguardientes</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+      <c r="D5">
+        <v>108000</v>
+      </c>
+      <c r="E5" t="str">
+        <v>7/2/2026</v>
+      </c>
+      <c r="F5">
         <v>78000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se realizan ajustes a novedades visuales en dashboard, inicio de proceso de reporteria en excel desde la vista de dashboard, inclusion de filtro para movimientos y actualizacion de inventario
</commit_message>
<xml_diff>
--- a/data/inventario.xlsx
+++ b/data/inventario.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,87 +424,667 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Cerveza Corona</v>
+        <v>Aguardiente Amarillo Caja</v>
       </c>
       <c r="B2" t="str">
-        <v>Cervezas</v>
+        <v>Aguardientes</v>
       </c>
       <c r="C2">
-        <v>982</v>
+        <v>100</v>
       </c>
       <c r="D2">
-        <v>10000</v>
+        <v>122000</v>
       </c>
       <c r="E2" t="str">
-        <v>31/1/2026</v>
+        <v>10/2/2026</v>
       </c>
       <c r="F2">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Ron viejo de caldas (5años) botella</v>
+        <v>Aguardiente Amarillo Media</v>
       </c>
       <c r="B3" t="str">
-        <v>Rones</v>
+        <v>Aguardientes</v>
       </c>
       <c r="C3">
-        <v>999</v>
+        <v>100</v>
       </c>
       <c r="D3">
-        <v>132000</v>
+        <v>70000</v>
       </c>
       <c r="E3" t="str">
-        <v>3/2/2026</v>
+        <v>10/2/2026</v>
       </c>
       <c r="F3">
-        <v>78000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Aguardiente Amarillo Media</v>
+        <v>Aguardiente Amarillo Botella</v>
       </c>
       <c r="B4" t="str">
         <v>Aguardientes</v>
       </c>
       <c r="C4">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="D4">
-        <v>70000</v>
+        <v>108000</v>
       </c>
       <c r="E4" t="str">
-        <v>6/2/2026</v>
+        <v>10/2/2026</v>
       </c>
       <c r="F4">
-        <v>39000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Aguardiente Amarillo Botella</v>
+        <v>Aguardiente Ligth Caja</v>
       </c>
       <c r="B5" t="str">
         <v>Aguardientes</v>
       </c>
       <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>110000</v>
+      </c>
+      <c r="E5" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Aguardiente Ligth Media</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Aguardientes</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>56000</v>
+      </c>
+      <c r="E6" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Aguardiente Ligth Botella</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Aguardientes</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>86000</v>
+      </c>
+      <c r="E7" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Aguardiente Ligth Cuarto</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Aguardientes</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>36000</v>
+      </c>
+      <c r="E8" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Aguardiente Cristal Caja</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Aguardientes</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>100000</v>
+      </c>
+      <c r="E9" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Aguardiente Cristal Media</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Aguardientes</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>54000</v>
+      </c>
+      <c r="E10" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Aguardiente Cristal Botella</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Aguardientes</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>86000</v>
+      </c>
+      <c r="E11" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Aguardiente Cristal Cuarto</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Aguardientes</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>36000</v>
+      </c>
+      <c r="E12" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Ron 8 años Media</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Rones</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>88000</v>
+      </c>
+      <c r="E13" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Ron 8 años Botella</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Rones</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>156000</v>
+      </c>
+      <c r="E14" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Ron 5 años Media</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Rones</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>78000</v>
+      </c>
+      <c r="E15" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Ron 5 años Botella</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Rones</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>132000</v>
+      </c>
+      <c r="E16" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Ron Tradicional Caja</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Rones</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>110000</v>
+      </c>
+      <c r="E17" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Ron Tradicional Media</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Rones</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>68000</v>
+      </c>
+      <c r="E18" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Ron Tradicional Botella</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Rones</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19">
+        <v>104000</v>
+      </c>
+      <c r="E19" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Ron Tradicional Cuarto</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Rones</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>38000</v>
+      </c>
+      <c r="E20" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Brandy Botella</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Brandy</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>140000</v>
+      </c>
+      <c r="E21" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Brandy Media</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Brandy</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>78000</v>
+      </c>
+      <c r="E22" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Cerveza Poker</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Cervezas</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>9000</v>
+      </c>
+      <c r="E23" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Cerveza Aguila Ligth</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Cervezas</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+      <c r="D24">
+        <v>9000</v>
+      </c>
+      <c r="E24" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Cerveza Corona</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Cervezas</v>
+      </c>
+      <c r="C25">
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="E25" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Cerveza Club Colombia</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Cervezas</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
+        <v>10000</v>
+      </c>
+      <c r="E26" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Buchanans Media</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Whisky</v>
+      </c>
+      <c r="C27">
+        <v>100</v>
+      </c>
+      <c r="D27">
+        <v>130000</v>
+      </c>
+      <c r="E27" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Black and White</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Whisky</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>74000</v>
+      </c>
+      <c r="E28" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Gatorade</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Hidratantes</v>
+      </c>
+      <c r="C29">
         <v>1000</v>
       </c>
-      <c r="D5">
-        <v>108000</v>
-      </c>
-      <c r="E5" t="str">
-        <v>7/2/2026</v>
-      </c>
-      <c r="F5">
-        <v>78000</v>
+      <c r="D29">
+        <v>6000</v>
+      </c>
+      <c r="E29" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Electrolit</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Hidratantes</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+      <c r="D30">
+        <v>10000</v>
+      </c>
+      <c r="E30" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Ginger Canada Dry</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Gaseosas</v>
+      </c>
+      <c r="C31">
+        <v>100</v>
+      </c>
+      <c r="D31">
+        <v>5000</v>
+      </c>
+      <c r="E31" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Agua Botella Grande</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Otros</v>
+      </c>
+      <c r="C32">
+        <v>100</v>
+      </c>
+      <c r="D32">
+        <v>5000</v>
+      </c>
+      <c r="E32" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Agua Botella Pequeña</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Otros</v>
+      </c>
+      <c r="C33">
+        <v>100</v>
+      </c>
+      <c r="D33">
+        <v>3000</v>
+      </c>
+      <c r="E33" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Soda</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Gaseosas</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>5000</v>
+      </c>
+      <c r="E34" t="str">
+        <v>10/2/2026</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F34"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>